<commit_message>
refactor: update poetry env docs and am working on converting csv rows to bill
</commit_message>
<xml_diff>
--- a/example-data.xlsx
+++ b/example-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crudnicky/Development/68thandMaine/Juno/juno-api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crudnicky/Development/68thandMaine/Juno/juno_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A5F58C-8F14-8C41-926F-FB3FBBF39874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EDFF98-8A7A-E14B-BDA7-9B08CF87D295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{42BE0E2D-B1D0-C042-B1A2-DEEACA68EFB5}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{42BE0E2D-B1D0-C042-B1A2-DEEACA68EFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="bill" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>_archived</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -504,19 +498,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2672286E-394E-4D47-BB5C-EA1922CD949D}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -547,378 +541,372 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="B2">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45140.520833333336</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>145</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45140.520833333336</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1080</v>
+      </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45141.364583333336</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>15.23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45142.680555555555</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="D3">
-        <v>1080</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1">
-        <v>45141.364583333336</v>
-      </c>
-      <c r="G3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>15.23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="1">
-        <v>45142.680555555555</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>20</v>
+      </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45143.465277777781</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>34.630000000000003</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45144.791666666664</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="B7">
+        <v>140.33000000000001</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45145.621527777781</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45146.402777777781</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>241</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45147.725694444445</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>134.05000000000001</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45148.510416666664</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>368.02</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45149.836805555555</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1">
-        <v>45143.465277777781</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>34.630000000000003</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45144.791666666664</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>140.33000000000001</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1">
-        <v>45145.621527777781</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1">
-        <v>45146.402777777781</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>241</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1">
-        <v>45147.725694444445</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>134.05000000000001</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="1">
-        <v>45148.510416666664</v>
-      </c>
-      <c r="G10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
+      <c r="B12">
+        <v>683.32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45150.659722222219</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="D11">
-        <v>368.02</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="1">
-        <v>45149.836805555555</v>
-      </c>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+      <c r="B13">
+        <v>500</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45151.440972222219</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="D12">
-        <v>683.32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1">
-        <v>45150.659722222219</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13">
-        <v>500</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="1">
-        <v>45151.440972222219</v>
-      </c>
-      <c r="G13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>170</v>
+      </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="D14">
-        <v>170</v>
+      <c r="D14" s="1">
+        <v>45152.760416666664</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="1">
-        <v>45152.760416666664</v>
-      </c>
-      <c r="G14" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>31.45</v>
+      </c>
       <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15">
-        <v>31.45</v>
+        <v>24</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45153.559027777781</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="1">
-        <v>45153.559027777781</v>
-      </c>
-      <c r="G15" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>600</v>
+      </c>
       <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="D16">
-        <v>600</v>
+      <c r="D16" s="1">
+        <v>45337.559027777781</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="1">
-        <v>45337.559027777781</v>
-      </c>
-      <c r="G16" t="s">
-        <v>35</v>
+      <c r="G16">
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>250</v>
+      </c>
       <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17">
-        <v>250</v>
-      </c>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="1">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1">
         <v>45153.559027777781</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>34</v>
+      <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="K17">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add script to seed the database
</commit_message>
<xml_diff>
--- a/example-data.xlsx
+++ b/example-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crudnicky/Development/68thandMaine/Juno/juno_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EDFF98-8A7A-E14B-BDA7-9B08CF87D295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94D6286E-823D-8647-AACB-9680CDD419F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{42BE0E2D-B1D0-C042-B1A2-DEEACA68EFB5}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,7 +553,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="1">
-        <v>45140.520833333336</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
@@ -576,7 +576,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="1">
-        <v>45141.364583333336</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -599,7 +599,7 @@
         <v>28</v>
       </c>
       <c r="D4" s="1">
-        <v>45142.680555555555</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
@@ -622,7 +622,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="1">
-        <v>45143.465277777781</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
@@ -645,7 +645,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="1">
-        <v>45144.791666666664</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -668,7 +668,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="1">
-        <v>45145.621527777781</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -691,7 +691,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="1">
-        <v>45146.402777777781</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
@@ -714,7 +714,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="1">
-        <v>45147.725694444445</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -737,7 +737,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="1">
-        <v>45148.510416666664</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
@@ -760,7 +760,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="1">
-        <v>45149.836805555555</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E11" t="s">
         <v>32</v>
@@ -783,7 +783,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="1">
-        <v>45150.659722222219</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -806,7 +806,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="1">
-        <v>45151.440972222219</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -829,7 +829,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="1">
-        <v>45152.760416666664</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E14" t="s">
         <v>32</v>
@@ -852,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="1">
-        <v>45153.559027777781</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
@@ -875,7 +875,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="1">
-        <v>45337.559027777781</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -898,7 +898,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="1">
-        <v>45153.559027777781</v>
+        <v>45147.012407407405</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
build: update example data source
</commit_message>
<xml_diff>
--- a/example-data.xlsx
+++ b/example-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crudnicky/Development/68thandMaine/Juno/juno_api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crudnicky/Development/Juno/juno_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C99C4-0CFD-3540-9FD0-6E4655742305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EAC009-0900-5941-9B24-0FF9CCD1E31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{42BE0E2D-B1D0-C042-B1A2-DEEACA68EFB5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{42BE0E2D-B1D0-C042-B1A2-DEEACA68EFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="bill" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -50,24 +50,9 @@
     <t>due_date</t>
   </si>
   <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>logo</t>
-  </si>
-  <si>
-    <t>recurring</t>
-  </si>
-  <si>
-    <t>payment_method</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>verizon</t>
   </si>
   <si>
@@ -134,16 +119,7 @@
     <t>car</t>
   </si>
   <si>
-    <t>monthly</t>
-  </si>
-  <si>
-    <t>bi-annually</t>
-  </si>
-  <si>
     <t>parking</t>
-  </si>
-  <si>
-    <t>140k</t>
   </si>
   <si>
     <t>Spotify</t>
@@ -153,20 +129,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -192,14 +158,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,19 +476,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2672286E-394E-4D47-BB5C-EA1922CD949D}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,451 +503,309 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2">
         <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1500</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>15.23</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>34.630000000000003</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>140.33000000000001</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>241</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>134.05000000000001</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>368.02</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>683.32</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>500</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>31.45</v>
       </c>
       <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45147.012407407405</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1">
-        <v>45147.012407407405</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>250</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <v>178</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1">
         <v>45147.012407407405</v>
       </c>
-      <c r="E18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="6">
+        <v>28</v>
+      </c>
+      <c r="B19">
         <v>10.99</v>
       </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24">
-        <v>94760</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <f>SUM(B2:B19)</f>
-        <v>4422.0200000000004</v>
-      </c>
-      <c r="D25" s="3">
-        <v>6915.56</v>
-      </c>
-      <c r="F25" s="4">
-        <v>4792.6400000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D26" s="3">
-        <f>D25-B25</f>
-        <v>2493.54</v>
-      </c>
-      <c r="F26" s="4">
-        <f>F25-B25</f>
-        <v>370.61999999999989</v>
-      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>